<commit_message>
First 3 TL models data and handdrawn, split images
</commit_message>
<xml_diff>
--- a/Transfer Learning Models.xlsx
+++ b/Transfer Learning Models.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natashasoldin/Documents/Personal/University/Fourth Year/First Semester/EEE4114F/Project/EEE4114F-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uctcloud-my.sharepoint.com/personal/jnsrya006_myuct_ac_za/Documents/4. Fourth Year/First Semester/EEE4114F/Project/EEE4114F-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB23388C-A7BF-8C44-B7EF-D93EEBC2D84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="8_{DB23388C-A7BF-8C44-B7EF-D93EEBC2D84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94B9ADA3-DADC-4D91-83D6-6389FD19DB7A}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="2680" windowWidth="28040" windowHeight="17440" xr2:uid="{419530FF-150D-FA47-AFBA-94DF5A43759C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{419530FF-150D-FA47-AFBA-94DF5A43759C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Model Name</t>
   </si>
@@ -48,6 +48,42 @@
   </si>
   <si>
     <t xml:space="preserve">Testing Accuracy </t>
+  </si>
+  <si>
+    <t>Training Loss</t>
+  </si>
+  <si>
+    <t>Validation Loss</t>
+  </si>
+  <si>
+    <t>Testing Loss</t>
+  </si>
+  <si>
+    <t>ResNet50</t>
+  </si>
+  <si>
+    <t>VGG16</t>
+  </si>
+  <si>
+    <t>InceptionV3</t>
+  </si>
+  <si>
+    <t>Testing Time</t>
+  </si>
+  <si>
+    <t>Average Time per Classification</t>
+  </si>
+  <si>
+    <t>Number of images</t>
+  </si>
+  <si>
+    <t>Train and Validation Time (s)</t>
+  </si>
+  <si>
+    <t>Number of Images</t>
+  </si>
+  <si>
+    <t>Time per image (tbc)</t>
   </si>
 </sst>
 </file>
@@ -399,21 +435,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66133F3-2240-8846-987D-29D3C00D6C6B}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.796875" customWidth="1"/>
+    <col min="4" max="4" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.796875" customWidth="1"/>
+    <col min="6" max="6" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="25.5" customWidth="1"/>
+    <col min="9" max="9" width="15.69921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,10 +462,167 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>0.98429999999999995</v>
+      </c>
+      <c r="C2">
+        <v>5.04E-2</v>
+      </c>
+      <c r="D2">
+        <v>0.95</v>
+      </c>
+      <c r="E2">
+        <v>0.24640000000000001</v>
+      </c>
+      <c r="I2">
+        <v>0.93330000000000002</v>
+      </c>
+      <c r="J2">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="L2">
+        <f>36*5</f>
+        <v>180</v>
+      </c>
+      <c r="M2">
+        <f>K2/L2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="D3">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="E3">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="F3">
+        <v>2343</v>
+      </c>
+      <c r="I3">
+        <v>0.9778</v>
+      </c>
+      <c r="J3">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="K3">
+        <v>113</v>
+      </c>
+      <c r="L3">
+        <v>180</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M7" si="0">K3/L3</f>
+        <v>0.62777777777777777</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>0.99409999999999998</v>
+      </c>
+      <c r="C4">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="D4">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="E4">
+        <v>0.80779999999999996</v>
+      </c>
+      <c r="F4">
+        <v>474</v>
+      </c>
+      <c r="I4">
+        <v>0.9556</v>
+      </c>
+      <c r="J4">
+        <v>0.72970000000000002</v>
+      </c>
+      <c r="K4">
+        <v>24</v>
+      </c>
+      <c r="L4">
+        <v>180</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L5">
+        <v>180</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L6">
+        <v>180</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L7">
+        <v>180</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add plots for all models and update excel file
</commit_message>
<xml_diff>
--- a/Transfer Learning Models.xlsx
+++ b/Transfer Learning Models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uctcloud-my.sharepoint.com/personal/jnsrya006_myuct_ac_za/Documents/4. Fourth Year/First Semester/EEE4114F/Project/EEE4114F-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{DB23388C-A7BF-8C44-B7EF-D93EEBC2D84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94B9ADA3-DADC-4D91-83D6-6389FD19DB7A}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="8_{DB23388C-A7BF-8C44-B7EF-D93EEBC2D84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAB8C8F5-F9F5-4124-9B28-0423F06F49D1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{419530FF-150D-FA47-AFBA-94DF5A43759C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Model Name</t>
   </si>
@@ -83,7 +83,19 @@
     <t>Number of Images</t>
   </si>
   <si>
-    <t>Time per image (tbc)</t>
+    <t>EfficientNetB7</t>
+  </si>
+  <si>
+    <t>VGG19</t>
+  </si>
+  <si>
+    <t>InceptionResNetV2</t>
+  </si>
+  <si>
+    <t>ResNet152</t>
+  </si>
+  <si>
+    <t>Time per image (s)</t>
   </si>
 </sst>
 </file>
@@ -136,6 +148,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -435,15 +451,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66133F3-2240-8846-987D-29D3C00D6C6B}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="163" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.8984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.796875" customWidth="1"/>
     <col min="4" max="4" width="17.796875" bestFit="1" customWidth="1"/>
@@ -452,6 +468,7 @@
     <col min="7" max="8" width="25.5" customWidth="1"/>
     <col min="9" max="9" width="15.69921875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -477,7 +494,7 @@
         <v>14</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
         <v>3</v>
@@ -511,11 +528,24 @@
       <c r="E2">
         <v>0.24640000000000001</v>
       </c>
+      <c r="F2">
+        <v>787</v>
+      </c>
+      <c r="G2">
+        <v>2700</v>
+      </c>
+      <c r="H2">
+        <f>F2/G2</f>
+        <v>0.29148148148148151</v>
+      </c>
       <c r="I2">
         <v>0.93330000000000002</v>
       </c>
       <c r="J2">
         <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="K2">
+        <v>39</v>
       </c>
       <c r="L2">
         <f>36*5</f>
@@ -523,106 +553,265 @@
       </c>
       <c r="M2">
         <f>K2/L2</f>
-        <v>0</v>
+        <v>0.21666666666666667</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0.99019999999999997</v>
       </c>
       <c r="C3">
-        <v>1.2999999999999999E-2</v>
+        <v>2.1399999999999999E-2</v>
       </c>
       <c r="D3">
-        <v>0.97499999999999998</v>
+        <v>0.93120000000000003</v>
       </c>
       <c r="E3">
-        <v>8.4000000000000005E-2</v>
+        <v>0.53320000000000001</v>
       </c>
       <c r="F3">
-        <v>2343</v>
+        <v>2091</v>
+      </c>
+      <c r="G3">
+        <v>2700</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H8" si="0">F3/G3</f>
+        <v>0.77444444444444449</v>
       </c>
       <c r="I3">
-        <v>0.9778</v>
+        <v>0.9556</v>
       </c>
       <c r="J3">
-        <v>6.9999999999999999E-4</v>
+        <v>0.251</v>
       </c>
       <c r="K3">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="L3">
         <v>180</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M7" si="0">K3/L3</f>
-        <v>0.62777777777777777</v>
+        <f>K3/L3</f>
+        <v>0.51111111111111107</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>0.99409999999999998</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>8.7800000000000003E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="D4">
-        <v>0.96250000000000002</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="E4">
-        <v>0.80779999999999996</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="F4">
-        <v>474</v>
+        <v>2343</v>
+      </c>
+      <c r="G4">
+        <v>2700</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>0.86777777777777776</v>
       </c>
       <c r="I4">
-        <v>0.9556</v>
+        <v>0.9778</v>
       </c>
       <c r="J4">
-        <v>0.72970000000000002</v>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="K4">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="L4">
         <v>180</v>
       </c>
       <c r="M4">
-        <f t="shared" si="0"/>
-        <v>0.13333333333333333</v>
+        <f t="shared" ref="M4:M10" si="1">K4/L4</f>
+        <v>0.62777777777777777</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>0.99609999999999999</v>
+      </c>
+      <c r="C5">
+        <v>1.89E-2</v>
+      </c>
+      <c r="D5">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="E5">
+        <v>0.16089999999999999</v>
+      </c>
+      <c r="F5">
+        <v>2690</v>
+      </c>
+      <c r="G5">
+        <v>2700</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>0.99629629629629635</v>
+      </c>
+      <c r="I5">
+        <v>0.98329999999999995</v>
+      </c>
+      <c r="J5">
+        <v>5.8400000000000001E-2</v>
+      </c>
+      <c r="K5">
+        <v>137</v>
+      </c>
       <c r="L5">
         <v>180</v>
       </c>
       <c r="M5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>K5/L5</f>
+        <v>0.76111111111111107</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1.8E-3</v>
+      </c>
+      <c r="D6">
+        <v>0.9375</v>
+      </c>
+      <c r="E6">
+        <v>0.8609</v>
+      </c>
+      <c r="F6">
+        <v>1196</v>
+      </c>
+      <c r="G6">
+        <v>2700</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>0.44296296296296295</v>
+      </c>
+      <c r="I6">
+        <v>0.95</v>
+      </c>
+      <c r="J6">
+        <v>0.51519999999999999</v>
+      </c>
+      <c r="K6">
+        <v>50</v>
+      </c>
       <c r="L6">
         <v>180</v>
       </c>
       <c r="M6">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>K6/L6</f>
+        <v>0.27777777777777779</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0.99409999999999998</v>
+      </c>
+      <c r="C7">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="D7">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="E7">
+        <v>0.80779999999999996</v>
+      </c>
+      <c r="F7">
+        <v>474</v>
+      </c>
+      <c r="G7">
+        <v>2700</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>0.17555555555555555</v>
+      </c>
+      <c r="I7">
+        <v>0.9556</v>
+      </c>
+      <c r="J7">
+        <v>0.72970000000000002</v>
+      </c>
+      <c r="K7">
+        <v>24</v>
+      </c>
       <c r="L7">
         <v>180</v>
       </c>
       <c r="M7">
+        <f t="shared" si="1"/>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="C8">
+        <v>1.9407000000000001</v>
+      </c>
+      <c r="D8">
+        <v>0.86870000000000003</v>
+      </c>
+      <c r="E8">
+        <v>1.46</v>
+      </c>
+      <c r="F8">
+        <v>2363</v>
+      </c>
+      <c r="G8">
+        <v>2700</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.87518518518518518</v>
+      </c>
+      <c r="I8">
+        <v>0.9</v>
+      </c>
+      <c r="J8">
+        <v>0.80359999999999998</v>
+      </c>
+      <c r="K8">
+        <v>111</v>
+      </c>
+      <c r="L8">
+        <v>180</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>0.6166666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>